<commit_message>
created basic module plates
</commit_message>
<xml_diff>
--- a/Mechanical/Modules/Dimensions.xlsx
+++ b/Mechanical/Modules/Dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimva\source\repos\BombSquad\Mechanical\Modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4BBB37-044F-4E73-8149-404722346CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D82C5C-F40F-45D0-A415-E733BA5FF2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Parameter name</t>
   </si>
@@ -71,21 +71,6 @@
     <t>Height of 1U in a standard 19inch rack</t>
   </si>
   <si>
-    <t>ModuleWidth</t>
-  </si>
-  <si>
-    <t>ModuleHeight</t>
-  </si>
-  <si>
-    <t>ModuleDepth</t>
-  </si>
-  <si>
-    <t>ModuleCaseThickness</t>
-  </si>
-  <si>
-    <t>ModuleBottomThickness</t>
-  </si>
-  <si>
     <t>Width of the module</t>
   </si>
   <si>
@@ -98,28 +83,58 @@
     <t>Thickness of the module</t>
   </si>
   <si>
-    <t>ModuleCaseSlotWidth</t>
-  </si>
-  <si>
     <t>Width of the slots to connect two panels together</t>
   </si>
   <si>
-    <t>ModuleCaseSlotDepth</t>
-  </si>
-  <si>
     <t>Depth of the slots to connect two panels together</t>
   </si>
   <si>
-    <t>ModuleConnectorWidth</t>
-  </si>
-  <si>
     <t>Width of the connector of the module</t>
   </si>
   <si>
     <t>Height of the connector of the module</t>
   </si>
   <si>
-    <t>ModuleConnectorDepth</t>
+    <t>Thickness back plate of the module</t>
+  </si>
+  <si>
+    <t>Module_Width</t>
+  </si>
+  <si>
+    <t>Module_Height</t>
+  </si>
+  <si>
+    <t>Module_Depth</t>
+  </si>
+  <si>
+    <t>Module_Case_Thickness</t>
+  </si>
+  <si>
+    <t>Module_Back_Thickness</t>
+  </si>
+  <si>
+    <t>Module_Case_SlotDepth</t>
+  </si>
+  <si>
+    <t>Module_Case_SlotWidth</t>
+  </si>
+  <si>
+    <t>Module_Connector_Width</t>
+  </si>
+  <si>
+    <t>Module_Connector_Depth</t>
+  </si>
+  <si>
+    <t>Module_StatusIndicatorDiameter</t>
+  </si>
+  <si>
+    <t>Diameter of the LED indicating the status of the module (good/bad/unsolved)</t>
+  </si>
+  <si>
+    <t>Module_Case_BottomSlotDepth</t>
+  </si>
+  <si>
+    <t>Depth of the slots to connect the side panels to the bottom panel</t>
   </si>
 </sst>
 </file>
@@ -446,16 +461,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -502,7 +517,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <f>RackWidth / 5</f>
@@ -512,12 +527,12 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <f>U * 2</f>
@@ -527,12 +542,12 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <f>50</f>
@@ -542,12 +557,12 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <f>3</f>
@@ -557,12 +572,12 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -576,7 +591,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <f>ModuleCaseThickness</f>
@@ -586,35 +601,36 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <f>ModuleBottomThickness</f>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,13 +638,41 @@
         <v>25</v>
       </c>
       <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>